<commit_message>
Reecriture de la classe décor
</commit_message>
<xml_diff>
--- a/documentation/avancement/taches.xlsx
+++ b/documentation/avancement/taches.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>TACHES</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>undefined</t>
+  </si>
+  <si>
+    <t>Remettre le code aux normes</t>
+  </si>
+  <si>
+    <t>Respecter les règles de nommage d'après le document</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>22</v>
@@ -654,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="9">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>24</v>
@@ -679,34 +685,34 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
+      <c r="A7" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>14</v>
@@ -714,17 +720,19 @@
       <c r="E8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>25</v>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -732,22 +740,20 @@
       <c r="E9" s="8">
         <v>0</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -758,11 +764,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>20</v>
@@ -770,20 +778,20 @@
       <c r="E11" s="8">
         <v>0</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>25</v>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -794,11 +802,11 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
@@ -812,16 +820,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -832,13 +838,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>20</v>
@@ -851,22 +857,42 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>